<commit_message>
docs: added updated product backlog and user stories
</commit_message>
<xml_diff>
--- a/docs/User Stories-1.xlsx
+++ b/docs/User Stories-1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamal\Desktop\Schoolwork\Summer 2025\ITSC 3155 (Software Engineering)\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamal\Desktop\Schoolwork\Summer 2025\ITSC 3155 (Software Engineering)\Group Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9DC7E5-6143-4C6D-BB00-993E4CD4389B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6F9FD3-BF5D-420F-8965-4E8C2DA01F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
   <si>
     <t>ITSC-3155 Software Engineering</t>
   </si>
@@ -52,238 +52,175 @@
     <t>STORY POINT</t>
   </si>
   <si>
-    <t>Customer-Facing API Platform</t>
-  </si>
-  <si>
-    <t>Restaurant Owner</t>
-  </si>
-  <si>
-    <t>Reach more customers through an online platform</t>
-  </si>
-  <si>
-    <t>I can boost my sales</t>
-  </si>
-  <si>
-    <t>As a restaurant owner, I want to reach more customers through an online platform so I can boost my sales.</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
-    <t>Online Ordering Interface</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Order food online</t>
-  </si>
-  <si>
-    <t>Enjoy meals without leaving home.</t>
-  </si>
-  <si>
-    <t>As a hungry customer, I want to browse and order food online so I can enjoy meals without leaving home.</t>
-  </si>
-  <si>
-    <t>Guest Checkout</t>
-  </si>
-  <si>
-    <t>First-Time user</t>
-  </si>
-  <si>
-    <t>Place an order without an account</t>
-  </si>
-  <si>
-    <t>I can quickly get my food.</t>
-  </si>
-  <si>
-    <t>As a first-time guest, I want to place an order without an account so I can quickly get my food.</t>
-  </si>
-  <si>
-    <t>Real-Time Order Tracking</t>
-  </si>
-  <si>
-    <t>Track my order using a tracking number</t>
-  </si>
-  <si>
-    <t>I know when to expect my food.</t>
-  </si>
-  <si>
-    <t>As a cutomer, I want to track my order using a tracking number so that I know when to expect my food.</t>
-  </si>
-  <si>
-    <t>Delivery/Takeout Options</t>
-  </si>
-  <si>
-    <t>Pick between delivery and takeout</t>
-  </si>
-  <si>
-    <t>I can decide how to receive my order.</t>
-  </si>
-  <si>
-    <t>As a customer, I want to pick between takeout and delivery so I can decide how I receive my order.</t>
-  </si>
-  <si>
-    <t>Menu Dislplay with Metadata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See detailed dish info </t>
-  </si>
-  <si>
-    <t>I can choose meals that fit my preferences.</t>
-  </si>
-  <si>
-    <t>As a customer, I want to see detailed dish info so I can choose meals that fit my preferences.</t>
-  </si>
-  <si>
     <t>Medium</t>
   </si>
   <si>
-    <t>Multi-Method Payment Gateway</t>
-  </si>
-  <si>
-    <t>Use various payment methods</t>
-  </si>
-  <si>
-    <t>I can pay the way I prefer</t>
-  </si>
-  <si>
-    <t>As a customer, I want to use various payment methods so I can pay the way I prefer.</t>
-  </si>
-  <si>
-    <t>Role-Based User Interfaces</t>
-  </si>
-  <si>
-    <t>Restaurant Staff</t>
-  </si>
-  <si>
-    <t>Use a dashboard tailored to my role</t>
-  </si>
-  <si>
-    <t>I can manage orders efficiently.</t>
-  </si>
-  <si>
-    <t>As restaurant staff, I want a dashboard tailored to my role so I can manage orders efficiently</t>
-  </si>
-  <si>
-    <t>Kitchen Order Display System</t>
-  </si>
-  <si>
-    <t>Chef</t>
-  </si>
-  <si>
-    <t>View incoming orders in real-time</t>
-  </si>
-  <si>
-    <t>I can start preparing food promptly.</t>
-  </si>
-  <si>
-    <t>As a chef, I want to view incoming orders in real-time so I can start preparing food promptly.</t>
-  </si>
-  <si>
-    <t>Admin Analytics Dashboard</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>See summarized operational data</t>
-  </si>
-  <si>
-    <t>I can monitor performance.</t>
-  </si>
-  <si>
-    <t>As an admin, I want to see summarized operational data so I can monitor performance.</t>
-  </si>
-  <si>
-    <t>Customer Review Module</t>
-  </si>
-  <si>
-    <t>Leave reviews and ratings after my meal</t>
-  </si>
-  <si>
-    <t>I can share my experience</t>
-  </si>
-  <si>
-    <t>As a customer, I want to leave reviews and ratings after my meal so I can share my experience.</t>
-  </si>
-  <si>
-    <t>Feedback Reporting System</t>
-  </si>
-  <si>
-    <t>Analyze customer feedback</t>
-  </si>
-  <si>
-    <t>I can improve menu items and service quality</t>
-  </si>
-  <si>
-    <t>As a restaurant owner, I want to analyze feedback so I can improve menu items and service quality.</t>
-  </si>
-  <si>
-    <t>Coupon/Promo Code Engine</t>
-  </si>
-  <si>
-    <t>Use promo codes when placing an order</t>
-  </si>
-  <si>
-    <t>Save money</t>
-  </si>
-  <si>
-    <t>As a customer, I want to use promo codes when placing an order so I can save money.</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
-    <t>Promotion Management Dashboard</t>
-  </si>
-  <si>
-    <t>Create and manage promotions</t>
-  </si>
-  <si>
-    <t>Attract more customers</t>
-  </si>
-  <si>
-    <t>As a restaurant owner, I want to create and manage promotions so I can attract more customers.</t>
-  </si>
-  <si>
-    <t>Data Analytics and Reporting Tools</t>
-  </si>
-  <si>
-    <t>View reports on order trends and customer preferences</t>
-  </si>
-  <si>
-    <t>Make informed business deccisions</t>
-  </si>
-  <si>
-    <t>As a restaurant owner, I want to view reports on order trends and customer preferences so I can make informed business decisions.</t>
-  </si>
-  <si>
-    <t>Integrated Training Resources</t>
-  </si>
-  <si>
-    <t>Have access to training materials</t>
-  </si>
-  <si>
-    <t>Learn how to use the system effectively.</t>
-  </si>
-  <si>
-    <t>As restaurant staff, I want access to training materials so I can learn how to use the system effectively.</t>
-  </si>
-  <si>
-    <t>System Documentation Repository</t>
-  </si>
-  <si>
-    <t>System Admin</t>
-  </si>
-  <si>
-    <t>Have comprehensive documentation</t>
-  </si>
-  <si>
-    <t>I can support and extend the platform in the future.</t>
-  </si>
-  <si>
-    <t>As a system admin, I want comprehensive documentation so I can support and extend the platform in the future.</t>
+    <t>As a guest customer, I want to place, pay for, and track orders without creating an account, so that I can quickly order food with minimal friction.</t>
+  </si>
+  <si>
+    <t>As a restaurant manager, I want to fully manage menu items and their properties, so that customers see accurate, up-to-date menu information.</t>
+  </si>
+  <si>
+    <t>As a kitchen manager, I want to track all ingredients and resources, so that I can prevent stockouts and optimize ordering.</t>
+  </si>
+  <si>
+    <t>As a restaurant staff member, I want to manage orders from placement to completion, so that customers receive accurate orders promptly.</t>
+  </si>
+  <si>
+    <t>As a kitchen staff member, I want to see detailed breakdown of each order, so that I can prepare items accurately.</t>
+  </si>
+  <si>
+    <t>As a customer and staff member, I want to process payments securely and efficiently, so that transactions are completed safely.</t>
+  </si>
+  <si>
+    <t>As a marketing manager, I want to create and manage promotional campaigns, so that I can drive sales and customer loyalty.</t>
+  </si>
+  <si>
+    <t>As a customer, I want to leave reviews and ratings for menu items, so that other customers can make informed choices.</t>
+  </si>
+  <si>
+    <t>As a restaurant manager, I want to access comprehensive business analytics, so that I can make data-driven decisions.</t>
+  </si>
+  <si>
+    <t>As a restaurant manager, I want to manage all staff operations efficiently, so that the restaurant runs smoothly.</t>
+  </si>
+  <si>
+    <t>As a system administrator, I want to manage the entire system infrastructure, so that the restaurant system operates reliably.</t>
+  </si>
+  <si>
+    <t>I can quickly order food with minimal friction</t>
+  </si>
+  <si>
+    <t>customers see accurate, up-to-date menu information</t>
+  </si>
+  <si>
+    <t>I can prevent stockouts and optimize ordering</t>
+  </si>
+  <si>
+    <t>customers receive accurate orders promptly</t>
+  </si>
+  <si>
+    <t>I can prepare items accurately</t>
+  </si>
+  <si>
+    <t>transactions are completed safely</t>
+  </si>
+  <si>
+    <t>I can drive sales and customer loyalty</t>
+  </si>
+  <si>
+    <t>I can make data-driven decisions</t>
+  </si>
+  <si>
+    <t>the restaurant runs smoothly</t>
+  </si>
+  <si>
+    <t>the restaurant system operates reliably</t>
+  </si>
+  <si>
+    <t>place, pay for, and track orders without creating an account</t>
+  </si>
+  <si>
+    <t>fully manage menu items and their properties</t>
+  </si>
+  <si>
+    <t>track all ingredients and resources</t>
+  </si>
+  <si>
+    <t>manage orders from placement to completion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> see detailed breakdown of each order</t>
+  </si>
+  <si>
+    <t>process payments securely and efficiently</t>
+  </si>
+  <si>
+    <t>create and manage promotional campaigns</t>
+  </si>
+  <si>
+    <t>access comprehensive business analytics</t>
+  </si>
+  <si>
+    <t>manage all staff operations efficiently</t>
+  </si>
+  <si>
+    <t>manage the entire system infrastructure</t>
+  </si>
+  <si>
+    <t>guest customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> restaurant manager</t>
+  </si>
+  <si>
+    <t>kitchen manager</t>
+  </si>
+  <si>
+    <t>restaurant staff member</t>
+  </si>
+  <si>
+    <t>kitchen staff member</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> customer and staff member</t>
+  </si>
+  <si>
+    <t>marketing manager</t>
+  </si>
+  <si>
+    <t>restaurant manager</t>
+  </si>
+  <si>
+    <t>system administrator</t>
+  </si>
+  <si>
+    <t>Guest Order Management System</t>
+  </si>
+  <si>
+    <t>Order Details Management</t>
+  </si>
+  <si>
+    <t>Order Processing Workflow</t>
+  </si>
+  <si>
+    <t>Inventory &amp; Resource Management</t>
+  </si>
+  <si>
+    <t>Menu Management System</t>
+  </si>
+  <si>
+    <t>Payment Processing System</t>
+  </si>
+  <si>
+    <t>Promotion Management System</t>
+  </si>
+  <si>
+    <t>Review and Rating System</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>leave reviews and ratings for menu items</t>
+  </si>
+  <si>
+    <t>other customers can make informed choices</t>
+  </si>
+  <si>
+    <t>Business Analytics Dashboard</t>
+  </si>
+  <si>
+    <t>Staff Management System</t>
+  </si>
+  <si>
+    <t>System Administration</t>
   </si>
 </sst>
 </file>
@@ -365,7 +302,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -447,35 +384,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -507,12 +420,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -747,34 +654,34 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -795,16 +702,16 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -868,30 +775,30 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="H4" s="10">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -912,30 +819,30 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5" s="10">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -956,30 +863,30 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10">
         <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="10">
-        <v>3</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1000,30 +907,30 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="C7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="10">
         <v>17</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="10">
-        <v>8</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1044,30 +951,30 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H8" s="10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1088,30 +995,30 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H9" s="10">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1132,27 +1039,27 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H10" s="10">
         <v>8</v>
@@ -1176,27 +1083,27 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="52.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H11" s="10">
         <v>8</v>
@@ -1225,25 +1132,25 @@
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H12" s="10">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1264,30 +1171,30 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="H13" s="10">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1308,30 +1215,30 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="66" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="H14" s="10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1352,31 +1259,15 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>12</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="10">
-        <v>5</v>
-      </c>
+    <row r="15" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1396,31 +1287,15 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>13</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="10">
-        <v>3</v>
-      </c>
+    <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1440,31 +1315,15 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>14</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H17" s="10">
-        <v>5</v>
-      </c>
+    <row r="17" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1484,139 +1343,91 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" spans="1:26" ht="66" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>15</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" s="10">
-        <v>8</v>
-      </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
-    </row>
-    <row r="19" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <v>16</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H19" s="10">
-        <v>2</v>
-      </c>
+    <row r="18" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+    </row>
+    <row r="19" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-    </row>
-    <row r="20" spans="1:26" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
-        <v>17</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="10">
-        <v>3</v>
-      </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-      <c r="S20" s="15"/>
-      <c r="T20" s="15"/>
-      <c r="U20" s="15"/>
-      <c r="V20" s="15"/>
-      <c r="W20" s="15"/>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
-      <c r="Z20" s="15"/>
-    </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+    </row>
+    <row r="20" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+    </row>
+    <row r="21" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1626,23 +1437,23 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -1896,7 +1707,34 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+    </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2866,13 +2704,14 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G20" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G4:G14" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>